<commit_message>
work on mobile automation task
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/yahooData.xlsx
+++ b/src/test/resources/xls/yahooData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Solvd\Carina\carina-demo\src\test\resources\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA2C3BB-C2E7-438F-A35C-18CAE670ED04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557FE43-45F4-4466-8EE4-68819EBCEC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{138A1EE6-55A2-4679-BF58-7AA87792B9D1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Execute</t>
   </si>
@@ -78,23 +78,41 @@
     <t>0</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>felipecopello94@gmail.com</t>
-  </si>
-  <si>
-    <t>notARobot</t>
-  </si>
-  <si>
-    <t>Demuestra que no eres un robot</t>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>expectedUrl</t>
+  </si>
+  <si>
+    <t>https://es.noticias.yahoo.com/</t>
+  </si>
+  <si>
+    <t>https://es.sports.yahoo.com/</t>
+  </si>
+  <si>
+    <t>https://es.finance.yahoo.com/</t>
+  </si>
+  <si>
+    <t>https://es.vida-estilo.yahoo.com/television/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Noticias   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deportes   </t>
+  </si>
+  <si>
+    <t>Finanzas</t>
+  </si>
+  <si>
+    <t>TV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +143,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,10 +169,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,8 +193,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,16 +607,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD277CCD-7E75-4352-A456-8555E01F0FCC}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="29.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,11 +628,11 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>16</v>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,15 +642,61 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{434D93FB-2C3E-4189-860A-AAEDA7C9C42F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>